<commit_message>
commit html reporter for tabs
</commit_message>
<xml_diff>
--- a/templates/Crosstab_Config_Template.xlsx
+++ b/templates/Crosstab_Config_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duncan/Documents/Turas/templates/Final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duncan/Documents/Turas/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893CD580-6A5A-964E-BD9D-732252BA1C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA559B7B-FECD-0449-AFCB-E439A5F02898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23740" windowHeight="25340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20600" yWindow="500" windowWidth="23740" windowHeight="25340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="257">
   <si>
     <t>Crosstab Configuration Template - Instructions</t>
   </si>
@@ -611,14 +611,444 @@
   <si>
     <t>Version 10.0 Last updated 4 December 2025</t>
   </si>
+  <si>
+    <t>HTML Summary</t>
+  </si>
+  <si>
+    <t>html_report</t>
+  </si>
+  <si>
+    <t>project_title</t>
+  </si>
+  <si>
+    <t>SACAP Student Annual 2025</t>
+  </si>
+  <si>
+    <t>brand_colour</t>
+  </si>
+  <si>
+    <t>#0d8a8a</t>
+  </si>
+  <si>
+    <t>include_summary</t>
+  </si>
+  <si>
+    <t>fieldwork_dates</t>
+  </si>
+  <si>
+    <t>Sep - Nov 2025</t>
+  </si>
+  <si>
+    <t>dashboard_metrics</t>
+  </si>
+  <si>
+    <t>NET POSITIVE, Index</t>
+  </si>
+  <si>
+    <t>dashboard_scale_index</t>
+  </si>
+  <si>
+    <t>dashboard_green_net</t>
+  </si>
+  <si>
+    <t>dashboard_amber_net</t>
+  </si>
+  <si>
+    <t>dashboard_green_index</t>
+  </si>
+  <si>
+    <t>dashboard_amber_index</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Which metric types to show</t>
+  </si>
+  <si>
+    <t>NET POSITIVE</t>
+  </si>
+  <si>
+    <t>Comma-separated list</t>
+  </si>
+  <si>
+    <t>See "Metric Types" below</t>
+  </si>
+  <si>
+    <t>dashboard_scale_mean</t>
+  </si>
+  <si>
+    <t>Max of the Mean gauge scale</t>
+  </si>
+  <si>
+    <r>
+      <t>Any number (e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF8A2424"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF3D3D3A"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF8A2424"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF3D3D3A"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Controls gauge arc fill</t>
+  </si>
+  <si>
+    <t>Max of the Index gauge scale</t>
+  </si>
+  <si>
+    <t>NET/NPS: green threshold</t>
+  </si>
+  <si>
+    <r>
+      <t>Any number (e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF8A2424"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF3D3D3A"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF8A2424"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>40</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF3D3D3A"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Value ≥ this = green</t>
+  </si>
+  <si>
+    <t>NET/NPS: amber threshold</t>
+  </si>
+  <si>
+    <r>
+      <t>Any number (e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF8A2424"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF3D3D3A"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF8A2424"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF3D3D3A"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Value ≥ this = amber</t>
+  </si>
+  <si>
+    <t>dashboard_green_mean</t>
+  </si>
+  <si>
+    <t>Mean: green threshold</t>
+  </si>
+  <si>
+    <t>Number on your scale</t>
+  </si>
+  <si>
+    <t>dashboard_amber_mean</t>
+  </si>
+  <si>
+    <t>Mean: amber threshold</t>
+  </si>
+  <si>
+    <t>Index: green threshold</t>
+  </si>
+  <si>
+    <t>Index: amber threshold</t>
+  </si>
+  <si>
+    <t>dashboard_green_custom</t>
+  </si>
+  <si>
+    <t>Custom %: green threshold</t>
+  </si>
+  <si>
+    <r>
+      <t>Percentage (e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF8A2424"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>60</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF3D3D3A"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF8A2424"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>70</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF3D3D3A"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>dashboard_amber_custom</t>
+  </si>
+  <si>
+    <r>
+      <t>Metric Types for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF8A2424"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>dashboard_metrics</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>These go in the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF8A2424"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>dashboard_metrics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF141413"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t> value, comma-separated:</t>
+    </r>
+  </si>
+  <si>
+    <t>What it matches</t>
+  </si>
+  <si>
+    <t>Value type</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Rows with "NET POSITIVE" in RowLabel, RowType = "Column %"</t>
+  </si>
+  <si>
+    <t>Percentage (can be negative)</t>
+  </si>
+  <si>
+    <t>-100 to +100 (fixed)</t>
+  </si>
+  <si>
+    <t>NPS</t>
+  </si>
+  <si>
+    <t>Rows with "NPS" in RowLabel, RowType = "Score" or "Average"</t>
+  </si>
+  <si>
+    <t>Score (can be negative)</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Rows with RowType = "Average"</t>
+  </si>
+  <si>
+    <t>Decimal number</t>
+  </si>
+  <si>
+    <r>
+      <t>0 to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF8A2424"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>dashboard_scale_mean</t>
+    </r>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Rows with RowType = "Index"</t>
+  </si>
+  <si>
+    <r>
+      <t>0 to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF8A2424"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>dashboard_scale_index</t>
+    </r>
+  </si>
+  <si>
+    <t>Any custom label</t>
+  </si>
+  <si>
+    <r>
+      <t>Matched against RowLabel (e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF8A2424"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Good or excellent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3D3D3A"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Column %</t>
+  </si>
+  <si>
+    <t>0 to 100%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -674,6 +1104,36 @@
       <i/>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF3D3D3A"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF8A2424"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF8A2424"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF141413"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3D3D3A"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -734,61 +1194,65 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{9871AC34-B7AD-FA4C-A159-6767873806FE}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1090,7 +1554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
@@ -1181,10 +1645,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1193,6 +1657,9 @@
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" customWidth="1"/>
     <col min="4" max="4" width="50.1640625" customWidth="1"/>
+    <col min="5" max="5" width="37" customWidth="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1969,6 +2436,457 @@
       </c>
       <c r="D60" s="8" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="B62" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B65" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="B66" s="25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="B67" s="25" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="B68" s="25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="B69" s="25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="B70" s="25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="B71" s="25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="B72" s="25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C74" s="4"/>
+      <c r="D74" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C75" s="4"/>
+      <c r="D75" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B76" s="4">
+        <v>10</v>
+      </c>
+      <c r="C76" s="4"/>
+      <c r="D76" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B77" s="4">
+        <v>10</v>
+      </c>
+      <c r="C77" s="4"/>
+      <c r="D77" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="G77" s="9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B78" s="4">
+        <v>30</v>
+      </c>
+      <c r="C78" s="4"/>
+      <c r="D78" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B79" s="4">
+        <v>0</v>
+      </c>
+      <c r="C79" s="4"/>
+      <c r="D79" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B80" s="4">
+        <v>7</v>
+      </c>
+      <c r="C80" s="4"/>
+      <c r="D80" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B81" s="4">
+        <v>5</v>
+      </c>
+      <c r="C81" s="4"/>
+      <c r="D81" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B82" s="4">
+        <v>7</v>
+      </c>
+      <c r="C82" s="4"/>
+      <c r="D82" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B83" s="4">
+        <v>5</v>
+      </c>
+      <c r="C83" s="4"/>
+      <c r="D83" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B84" s="4">
+        <v>60</v>
+      </c>
+      <c r="C84" s="4"/>
+      <c r="D84" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B85" s="4">
+        <v>60</v>
+      </c>
+      <c r="C85" s="4"/>
+      <c r="D85" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9"/>
+    </row>
+    <row r="91" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="D91" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="9"/>
+    </row>
+    <row r="92" spans="1:7" ht="38" x14ac:dyDescent="0.2">
+      <c r="D92" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+    </row>
+    <row r="93" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="D93" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="G93" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="D94" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="G94" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="D95" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="G95" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="D96" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="G96" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="97" spans="4:7" ht="52" x14ac:dyDescent="0.2">
+      <c r="D97" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="G97" s="9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="98" spans="4:7" ht="36" x14ac:dyDescent="0.2">
+      <c r="D98" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="G98" s="9" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>